<commit_message>
Fiscal Quarter and pricing/veh title fixes.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Customer/Air_Force/Air_Force_Contracts.xlsx
+++ b/Output/AcqTrends/Customer/Air_Force/Air_Force_Contracts.xlsx
@@ -9,12 +9,14 @@
     <sheet name="PSR" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Plat" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Price" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="FYQ" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Veh" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t xml:space="preserve">SimpleArea</t>
   </si>
@@ -211,19 +213,60 @@
     <t xml:space="preserve">Undefinitized
 Contract Award</t>
   </si>
+  <si>
+    <t xml:space="preserve">Vehicle.AwardTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle.sum7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Award</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pur. Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOA or BPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSS or GWAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Awd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Awd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unlbd. IDV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00,,,&quot;B&quot;"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -246,8 +289,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5926,4 +5971,3398 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="2" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1" t="n">
+        <v>25037791820.28</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>25987627628.125</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>30299261383.9775</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>32207058151.3866</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <v>30328711951.8153</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>27829791611.4059</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>32177683976.4133</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>34883515514.1267</v>
+      </c>
+      <c r="AG2" s="1" t="n">
+        <v>31027929889.2513</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>32875058064.4656</v>
+      </c>
+      <c r="AI2" s="1" t="n">
+        <v>30416463887.6224</v>
+      </c>
+      <c r="AJ2" s="1" t="n">
+        <v>32442032021.952</v>
+      </c>
+      <c r="AK2" s="1" t="n">
+        <v>36243285201.6863</v>
+      </c>
+      <c r="AL2" s="1" t="n">
+        <v>28738866549.7774</v>
+      </c>
+      <c r="AM2" s="1" t="n">
+        <v>29224642112.3227</v>
+      </c>
+      <c r="AN2" s="1" t="n">
+        <v>26728714114.7883</v>
+      </c>
+      <c r="AO2" s="1" t="n">
+        <v>35382047605.571</v>
+      </c>
+      <c r="AP2" s="1" t="n">
+        <v>28839227430.4421</v>
+      </c>
+      <c r="AQ2" s="1" t="n">
+        <v>32185609526.1376</v>
+      </c>
+      <c r="AR2" s="1" t="n">
+        <v>32232730048.8324</v>
+      </c>
+      <c r="AS2" s="1" t="n">
+        <v>27888874191.2234</v>
+      </c>
+      <c r="AT2" s="1" t="n">
+        <v>32293940253.82</v>
+      </c>
+      <c r="AU2" s="1" t="n">
+        <v>29109738531.2029</v>
+      </c>
+      <c r="AV2" s="1" t="n">
+        <v>19266830668.5575</v>
+      </c>
+      <c r="AW2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="M3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1" t="n">
+        <v>429991936</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>462457544</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>580716042.8604</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>814693170.4201</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>699659535.1131</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>905201048.2908</v>
+      </c>
+      <c r="AE3" s="1" t="n">
+        <v>1009097304.2691</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>1104709717.6857</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>1031110140.2592</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>1048622648.7144</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>993249631.0746</v>
+      </c>
+      <c r="AJ3" s="1" t="n">
+        <v>974754574.7314</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>754192638.8197</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>585889371.8041</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>708079176.1999</v>
+      </c>
+      <c r="AN3" s="1" t="n">
+        <v>654096032.3745</v>
+      </c>
+      <c r="AO3" s="1" t="n">
+        <v>718615400.6798</v>
+      </c>
+      <c r="AP3" s="1" t="n">
+        <v>770474048.8266</v>
+      </c>
+      <c r="AQ3" s="1" t="n">
+        <v>836529128.8416</v>
+      </c>
+      <c r="AR3" s="1" t="n">
+        <v>970251135.2166</v>
+      </c>
+      <c r="AS3" s="1" t="n">
+        <v>1059955437.244</v>
+      </c>
+      <c r="AT3" s="1" t="n">
+        <v>1378269878.9255</v>
+      </c>
+      <c r="AU3" s="1" t="n">
+        <v>1586761989.3851</v>
+      </c>
+      <c r="AV3" s="1" t="n">
+        <v>605325076.8962</v>
+      </c>
+      <c r="AW3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="M4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1" t="n">
+        <v>794993</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>5766024</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <v>18457363</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <v>21048810</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>8333396</v>
+      </c>
+      <c r="AD4" s="1" t="n">
+        <v>7380604</v>
+      </c>
+      <c r="AE4" s="1" t="n">
+        <v>8035145</v>
+      </c>
+      <c r="AF4" s="1" t="n">
+        <v>2593749.5782</v>
+      </c>
+      <c r="AG4" s="1" t="n">
+        <v>3037136.4004</v>
+      </c>
+      <c r="AH4" s="1" t="n">
+        <v>-191.57</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>80526041.4074</v>
+      </c>
+      <c r="AJ4" s="1" t="n">
+        <v>1205687097.1125</v>
+      </c>
+      <c r="AK4" s="1" t="n">
+        <v>3785228474.7754</v>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>3588830488.7816</v>
+      </c>
+      <c r="AM4" s="1" t="n">
+        <v>3547464959.5712</v>
+      </c>
+      <c r="AN4" s="1" t="n">
+        <v>4158248013.9978</v>
+      </c>
+      <c r="AO4" s="1" t="n">
+        <v>4079140178.3866</v>
+      </c>
+      <c r="AP4" s="1" t="n">
+        <v>4331574462.2964</v>
+      </c>
+      <c r="AQ4" s="1" t="n">
+        <v>4814361963.939</v>
+      </c>
+      <c r="AR4" s="1" t="n">
+        <v>5165041167.6537</v>
+      </c>
+      <c r="AS4" s="1" t="n">
+        <v>4039210682.0812</v>
+      </c>
+      <c r="AT4" s="1" t="n">
+        <v>4181022951.238</v>
+      </c>
+      <c r="AU4" s="1" t="n">
+        <v>4135689645.2253</v>
+      </c>
+      <c r="AV4" s="1" t="n">
+        <v>2810193207.7628</v>
+      </c>
+      <c r="AW4" s="1"/>
+    </row>
+    <row r="5">
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1" t="n">
+        <v>1167331912</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>1676747428.4924</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>2117718162.5801</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>2882510310.7922</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <v>3000071367.2545</v>
+      </c>
+      <c r="AD5" s="1" t="n">
+        <v>3143873186.8138</v>
+      </c>
+      <c r="AE5" s="1" t="n">
+        <v>3315801109.2555</v>
+      </c>
+      <c r="AF5" s="1" t="n">
+        <v>2786606127.6962</v>
+      </c>
+      <c r="AG5" s="1" t="n">
+        <v>2397916048.7393</v>
+      </c>
+      <c r="AH5" s="1" t="n">
+        <v>2312431378.2869</v>
+      </c>
+      <c r="AI5" s="1" t="n">
+        <v>1879357769.5313</v>
+      </c>
+      <c r="AJ5" s="1" t="n">
+        <v>1578069327.0811</v>
+      </c>
+      <c r="AK5" s="1" t="n">
+        <v>1462436345.3911</v>
+      </c>
+      <c r="AL5" s="1" t="n">
+        <v>964787397.5667</v>
+      </c>
+      <c r="AM5" s="1" t="n">
+        <v>1259044409.1743</v>
+      </c>
+      <c r="AN5" s="1" t="n">
+        <v>993691370.6567</v>
+      </c>
+      <c r="AO5" s="1" t="n">
+        <v>1221989460.6681</v>
+      </c>
+      <c r="AP5" s="1" t="n">
+        <v>1064078503.0135</v>
+      </c>
+      <c r="AQ5" s="1" t="n">
+        <v>1342936841.4755</v>
+      </c>
+      <c r="AR5" s="1" t="n">
+        <v>1389286463.4796</v>
+      </c>
+      <c r="AS5" s="1" t="n">
+        <v>2176356701.8175</v>
+      </c>
+      <c r="AT5" s="1" t="n">
+        <v>1985876952.3088</v>
+      </c>
+      <c r="AU5" s="1" t="n">
+        <v>2086575759.0228</v>
+      </c>
+      <c r="AV5" s="1" t="n">
+        <v>881360650.0195</v>
+      </c>
+      <c r="AW5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="M6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1" t="n">
+        <v>2320173951</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>2729937455</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <v>3526006911.2676</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>5790650834.9219</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>6758654015.125</v>
+      </c>
+      <c r="AD6" s="1" t="n">
+        <v>7666611064.2898</v>
+      </c>
+      <c r="AE6" s="1" t="n">
+        <v>8427156969.5412</v>
+      </c>
+      <c r="AF6" s="1" t="n">
+        <v>9399128455.1433</v>
+      </c>
+      <c r="AG6" s="1" t="n">
+        <v>6830206594.959</v>
+      </c>
+      <c r="AH6" s="1" t="n">
+        <v>7451026417.8535</v>
+      </c>
+      <c r="AI6" s="1" t="n">
+        <v>6948176906.6676</v>
+      </c>
+      <c r="AJ6" s="1" t="n">
+        <v>6777124492.4024</v>
+      </c>
+      <c r="AK6" s="1" t="n">
+        <v>5403440476.1178</v>
+      </c>
+      <c r="AL6" s="1" t="n">
+        <v>4355883264.0082</v>
+      </c>
+      <c r="AM6" s="1" t="n">
+        <v>4557892835.049</v>
+      </c>
+      <c r="AN6" s="1" t="n">
+        <v>5546452743.2363</v>
+      </c>
+      <c r="AO6" s="1" t="n">
+        <v>6844533124.3459</v>
+      </c>
+      <c r="AP6" s="1" t="n">
+        <v>8572838086.3563</v>
+      </c>
+      <c r="AQ6" s="1" t="n">
+        <v>9431813502.821</v>
+      </c>
+      <c r="AR6" s="1" t="n">
+        <v>11043379299.655</v>
+      </c>
+      <c r="AS6" s="1" t="n">
+        <v>11792177479.1521</v>
+      </c>
+      <c r="AT6" s="1" t="n">
+        <v>11743892048.6738</v>
+      </c>
+      <c r="AU6" s="1" t="n">
+        <v>14075110863.4924</v>
+      </c>
+      <c r="AV6" s="1" t="n">
+        <v>6224661006.7286</v>
+      </c>
+      <c r="AW6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1" t="n">
+        <v>7854698435</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <v>9522931884.9922</v>
+      </c>
+      <c r="AA7" s="1" t="n">
+        <v>10700806025.8984</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>13663611137.4668</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>14163933177.4563</v>
+      </c>
+      <c r="AD7" s="1" t="n">
+        <v>15901650491.4803</v>
+      </c>
+      <c r="AE7" s="1" t="n">
+        <v>18167649663.3896</v>
+      </c>
+      <c r="AF7" s="1" t="n">
+        <v>21677474869.1647</v>
+      </c>
+      <c r="AG7" s="1" t="n">
+        <v>22352495458.8577</v>
+      </c>
+      <c r="AH7" s="1" t="n">
+        <v>24122206299.4763</v>
+      </c>
+      <c r="AI7" s="1" t="n">
+        <v>24344266986.4574</v>
+      </c>
+      <c r="AJ7" s="1" t="n">
+        <v>22300905029.3058</v>
+      </c>
+      <c r="AK7" s="1" t="n">
+        <v>23583134638.5674</v>
+      </c>
+      <c r="AL7" s="1" t="n">
+        <v>16718271014.0538</v>
+      </c>
+      <c r="AM7" s="1" t="n">
+        <v>16399652239.6038</v>
+      </c>
+      <c r="AN7" s="1" t="n">
+        <v>14788790206.1206</v>
+      </c>
+      <c r="AO7" s="1" t="n">
+        <v>16841532236.8939</v>
+      </c>
+      <c r="AP7" s="1" t="n">
+        <v>17399545625.617</v>
+      </c>
+      <c r="AQ7" s="1" t="n">
+        <v>22729246769.6889</v>
+      </c>
+      <c r="AR7" s="1" t="n">
+        <v>25045714764.7329</v>
+      </c>
+      <c r="AS7" s="1" t="n">
+        <v>31061800889.3761</v>
+      </c>
+      <c r="AT7" s="1" t="n">
+        <v>27470707824.7053</v>
+      </c>
+      <c r="AU7" s="1" t="n">
+        <v>27976052355.6285</v>
+      </c>
+      <c r="AV7" s="1" t="n">
+        <v>15915777194.386</v>
+      </c>
+      <c r="AW7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1" t="n">
+        <v>1148119396.6992</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <v>247578587</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <v>170918844.5508</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <v>177562642</v>
+      </c>
+      <c r="AC8" s="1" t="n">
+        <v>97332309</v>
+      </c>
+      <c r="AD8" s="1" t="n">
+        <v>125448697.2969</v>
+      </c>
+      <c r="AE8" s="1" t="n">
+        <v>34019384</v>
+      </c>
+      <c r="AF8" s="1" t="n">
+        <v>23108672.0863</v>
+      </c>
+      <c r="AG8" s="1" t="n">
+        <v>7962497.2337</v>
+      </c>
+      <c r="AH8" s="1" t="n">
+        <v>874136.2752</v>
+      </c>
+      <c r="AI8" s="1" t="n">
+        <v>243644521.7326</v>
+      </c>
+      <c r="AJ8" s="1" t="n">
+        <v>192890355.3557</v>
+      </c>
+      <c r="AK8" s="1" t="n">
+        <v>261626622.9468</v>
+      </c>
+      <c r="AL8" s="1" t="n">
+        <v>109962590.1993</v>
+      </c>
+      <c r="AM8" s="1" t="n">
+        <v>111679969.1173</v>
+      </c>
+      <c r="AN8" s="1" t="n">
+        <v>90863531.3495</v>
+      </c>
+      <c r="AO8" s="1" t="n">
+        <v>255428.6954</v>
+      </c>
+      <c r="AP8" s="1" t="n">
+        <v>26106440.6765</v>
+      </c>
+      <c r="AQ8" s="1" t="n">
+        <v>1930135.2498</v>
+      </c>
+      <c r="AR8" s="1" t="n">
+        <v>29285</v>
+      </c>
+      <c r="AS8" s="1" t="n">
+        <v>88463</v>
+      </c>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9" s="1" t="n">
+        <v>41032316000</v>
+      </c>
+      <c r="P9" s="1" t="n">
+        <v>43625084000</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>38602723036</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>39452449414</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>43554730825</v>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>37076749369</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <v>39081089944</v>
+      </c>
+      <c r="V9" s="1" t="n">
+        <v>34943056076</v>
+      </c>
+      <c r="W9" s="1" t="n">
+        <v>33653688998</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>35246060466</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="1"/>
+    </row>
+    <row r="13">
+      <c r="M13" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" t="s">
+        <v>5</v>
+      </c>
+      <c r="T13" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>68</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1" t="n">
+        <v>40454312623.8912</v>
+      </c>
+      <c r="Z14" s="1" t="n">
+        <v>40994888501.0211</v>
+      </c>
+      <c r="AA14" s="1" t="n">
+        <v>47053717919.2218</v>
+      </c>
+      <c r="AB14" s="1" t="n">
+        <v>49078349890.365</v>
+      </c>
+      <c r="AC14" s="1" t="n">
+        <v>45113332093.9883</v>
+      </c>
+      <c r="AD14" s="1" t="n">
+        <v>40176609630.433</v>
+      </c>
+      <c r="AE14" s="1" t="n">
+        <v>44988739214.7108</v>
+      </c>
+      <c r="AF14" s="1" t="n">
+        <v>47470078975.0205</v>
+      </c>
+      <c r="AG14" s="1" t="n">
+        <v>41360719904.0871</v>
+      </c>
+      <c r="AH14" s="1" t="n">
+        <v>43382123699.1001</v>
+      </c>
+      <c r="AI14" s="1" t="n">
+        <v>39791661083.1474</v>
+      </c>
+      <c r="AJ14" s="1" t="n">
+        <v>41603106829.4826</v>
+      </c>
+      <c r="AK14" s="1" t="n">
+        <v>45641169045.7752</v>
+      </c>
+      <c r="AL14" s="1" t="n">
+        <v>35540464136.3503</v>
+      </c>
+      <c r="AM14" s="1" t="n">
+        <v>35455290770.3958</v>
+      </c>
+      <c r="AN14" s="1" t="n">
+        <v>32059691116.0415</v>
+      </c>
+      <c r="AO14" s="1" t="n">
+        <v>42090130903.2132</v>
+      </c>
+      <c r="AP14" s="1" t="n">
+        <v>33705094312.0825</v>
+      </c>
+      <c r="AQ14" s="1" t="n">
+        <v>36753117584.409</v>
+      </c>
+      <c r="AR14" s="1" t="n">
+        <v>36099854996.0764</v>
+      </c>
+      <c r="AS14" s="1" t="n">
+        <v>30823643398.4323</v>
+      </c>
+      <c r="AT14" s="1" t="n">
+        <v>34531509704.6361</v>
+      </c>
+      <c r="AU14" s="1" t="n">
+        <v>29109738531.2029</v>
+      </c>
+      <c r="AV14" s="1" t="n">
+        <v>18376671868.5249</v>
+      </c>
+      <c r="AW14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1" t="n">
+        <v>694750892.153622</v>
+      </c>
+      <c r="Z15" s="1" t="n">
+        <v>729516203.788391</v>
+      </c>
+      <c r="AA15" s="1" t="n">
+        <v>901832177.545081</v>
+      </c>
+      <c r="AB15" s="1" t="n">
+        <v>1241460684.89795</v>
+      </c>
+      <c r="AC15" s="1" t="n">
+        <v>1040729095.59859</v>
+      </c>
+      <c r="AD15" s="1" t="n">
+        <v>1306797753.35914</v>
+      </c>
+      <c r="AE15" s="1" t="n">
+        <v>1410854040.87216</v>
+      </c>
+      <c r="AF15" s="1" t="n">
+        <v>1503307701.93663</v>
+      </c>
+      <c r="AG15" s="1" t="n">
+        <v>1374486079.27591</v>
+      </c>
+      <c r="AH15" s="1" t="n">
+        <v>1383768733.45746</v>
+      </c>
+      <c r="AI15" s="1" t="n">
+        <v>1299396696.36499</v>
+      </c>
+      <c r="AJ15" s="1" t="n">
+        <v>1250008590.01795</v>
+      </c>
+      <c r="AK15" s="1" t="n">
+        <v>949754789.884435</v>
+      </c>
+      <c r="AL15" s="1" t="n">
+        <v>724551198.649611</v>
+      </c>
+      <c r="AM15" s="1" t="n">
+        <v>859040565.292127</v>
+      </c>
+      <c r="AN15" s="1" t="n">
+        <v>784553894.665383</v>
+      </c>
+      <c r="AO15" s="1" t="n">
+        <v>854857712.613427</v>
+      </c>
+      <c r="AP15" s="1" t="n">
+        <v>900471434.033643</v>
+      </c>
+      <c r="AQ15" s="1" t="n">
+        <v>955242230.541908</v>
+      </c>
+      <c r="AR15" s="1" t="n">
+        <v>1086657110.27374</v>
+      </c>
+      <c r="AS15" s="1" t="n">
+        <v>1171495421.14254</v>
+      </c>
+      <c r="AT15" s="1" t="n">
+        <v>1473766883.99285</v>
+      </c>
+      <c r="AU15" s="1" t="n">
+        <v>1586761989.3851</v>
+      </c>
+      <c r="AV15" s="1" t="n">
+        <v>577358077.375156</v>
+      </c>
+      <c r="AW15" s="1"/>
+    </row>
+    <row r="16">
+      <c r="M16" t="s">
+        <v>70</v>
+      </c>
+      <c r="N16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1" t="n">
+        <v>1284494.07945614</v>
+      </c>
+      <c r="Z16" s="1" t="n">
+        <v>9095771.04754237</v>
+      </c>
+      <c r="AA16" s="1" t="n">
+        <v>28663654.2432003</v>
+      </c>
+      <c r="AB16" s="1" t="n">
+        <v>32074983.5983185</v>
+      </c>
+      <c r="AC16" s="1" t="n">
+        <v>12395754.2877521</v>
+      </c>
+      <c r="AD16" s="1" t="n">
+        <v>10655043.6986845</v>
+      </c>
+      <c r="AE16" s="1" t="n">
+        <v>11234215.7136718</v>
+      </c>
+      <c r="AF16" s="1" t="n">
+        <v>3529618.37429253</v>
+      </c>
+      <c r="AG16" s="1" t="n">
+        <v>4048550.72239184</v>
+      </c>
+      <c r="AH16" s="1" t="n">
+        <v>-252.796920411209</v>
+      </c>
+      <c r="AI16" s="1" t="n">
+        <v>105346399.235931</v>
+      </c>
+      <c r="AJ16" s="1" t="n">
+        <v>1546152505.80355</v>
+      </c>
+      <c r="AK16" s="1" t="n">
+        <v>4766738217.37517</v>
+      </c>
+      <c r="AL16" s="1" t="n">
+        <v>4438195259.26888</v>
+      </c>
+      <c r="AM16" s="1" t="n">
+        <v>4303779021.68914</v>
+      </c>
+      <c r="AN16" s="1" t="n">
+        <v>4987600463.68652</v>
+      </c>
+      <c r="AO16" s="1" t="n">
+        <v>4852504467.65594</v>
+      </c>
+      <c r="AP16" s="1" t="n">
+        <v>5062414592.19526</v>
+      </c>
+      <c r="AQ16" s="1" t="n">
+        <v>5497575281.61345</v>
+      </c>
+      <c r="AR16" s="1" t="n">
+        <v>5784717488.04963</v>
+      </c>
+      <c r="AS16" s="1" t="n">
+        <v>4464260149.83389</v>
+      </c>
+      <c r="AT16" s="1" t="n">
+        <v>4470715975.85256</v>
+      </c>
+      <c r="AU16" s="1" t="n">
+        <v>4135689645.2253</v>
+      </c>
+      <c r="AV16" s="1" t="n">
+        <v>2680357727.4643</v>
+      </c>
+      <c r="AW16" s="1"/>
+    </row>
+    <row r="17">
+      <c r="M17" t="s">
+        <v>70</v>
+      </c>
+      <c r="N17" t="s">
+        <v>72</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1" t="n">
+        <v>1886093248.2729</v>
+      </c>
+      <c r="Z17" s="1" t="n">
+        <v>2645030737.66642</v>
+      </c>
+      <c r="AA17" s="1" t="n">
+        <v>3288743966.12027</v>
+      </c>
+      <c r="AB17" s="1" t="n">
+        <v>4392479714.56076</v>
+      </c>
+      <c r="AC17" s="1" t="n">
+        <v>4462544143.37293</v>
+      </c>
+      <c r="AD17" s="1" t="n">
+        <v>4538667321.62076</v>
+      </c>
+      <c r="AE17" s="1" t="n">
+        <v>4635936865.48388</v>
+      </c>
+      <c r="AF17" s="1" t="n">
+        <v>3792060834.59235</v>
+      </c>
+      <c r="AG17" s="1" t="n">
+        <v>3196459912.06713</v>
+      </c>
+      <c r="AH17" s="1" t="n">
+        <v>3051498309.1986</v>
+      </c>
+      <c r="AI17" s="1" t="n">
+        <v>2458627922.54432</v>
+      </c>
+      <c r="AJ17" s="1" t="n">
+        <v>2023689106.60284</v>
+      </c>
+      <c r="AK17" s="1" t="n">
+        <v>1841646089.39963</v>
+      </c>
+      <c r="AL17" s="1" t="n">
+        <v>1193122625.17492</v>
+      </c>
+      <c r="AM17" s="1" t="n">
+        <v>1527470736.80308</v>
+      </c>
+      <c r="AN17" s="1" t="n">
+        <v>1191880696.95818</v>
+      </c>
+      <c r="AO17" s="1" t="n">
+        <v>1453666473.32668</v>
+      </c>
+      <c r="AP17" s="1" t="n">
+        <v>1243613976.34637</v>
+      </c>
+      <c r="AQ17" s="1" t="n">
+        <v>1533515020.21739</v>
+      </c>
+      <c r="AR17" s="1" t="n">
+        <v>1555966243.12132</v>
+      </c>
+      <c r="AS17" s="1" t="n">
+        <v>2405376510.52698</v>
+      </c>
+      <c r="AT17" s="1" t="n">
+        <v>2123473590.14987</v>
+      </c>
+      <c r="AU17" s="1" t="n">
+        <v>2086575759.0228</v>
+      </c>
+      <c r="AV17" s="1" t="n">
+        <v>840640359.686659</v>
+      </c>
+      <c r="AW17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="M18" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1" t="n">
+        <v>3748774773.32236</v>
+      </c>
+      <c r="Z18" s="1" t="n">
+        <v>4306413928.34829</v>
+      </c>
+      <c r="AA18" s="1" t="n">
+        <v>5475768286.27736</v>
+      </c>
+      <c r="AB18" s="1" t="n">
+        <v>8824015730.7567</v>
+      </c>
+      <c r="AC18" s="1" t="n">
+        <v>10053358137.2371</v>
+      </c>
+      <c r="AD18" s="1" t="n">
+        <v>11067939143.033</v>
+      </c>
+      <c r="AE18" s="1" t="n">
+        <v>11782301283.7725</v>
+      </c>
+      <c r="AF18" s="1" t="n">
+        <v>12790493259.8128</v>
+      </c>
+      <c r="AG18" s="1" t="n">
+        <v>9104773114.72243</v>
+      </c>
+      <c r="AH18" s="1" t="n">
+        <v>9832419127.92154</v>
+      </c>
+      <c r="AI18" s="1" t="n">
+        <v>9089797605.57828</v>
+      </c>
+      <c r="AJ18" s="1" t="n">
+        <v>8690868502.42111</v>
+      </c>
+      <c r="AK18" s="1" t="n">
+        <v>6804552590.27684</v>
+      </c>
+      <c r="AL18" s="1" t="n">
+        <v>5386785615.16933</v>
+      </c>
+      <c r="AM18" s="1" t="n">
+        <v>5529628562.9731</v>
+      </c>
+      <c r="AN18" s="1" t="n">
+        <v>6652679248.77445</v>
+      </c>
+      <c r="AO18" s="1" t="n">
+        <v>8142188331.96465</v>
+      </c>
+      <c r="AP18" s="1" t="n">
+        <v>10019280749.4504</v>
+      </c>
+      <c r="AQ18" s="1" t="n">
+        <v>10770296284.8004</v>
+      </c>
+      <c r="AR18" s="1" t="n">
+        <v>12368309813.6659</v>
+      </c>
+      <c r="AS18" s="1" t="n">
+        <v>13033078030.1915</v>
+      </c>
+      <c r="AT18" s="1" t="n">
+        <v>12557598083.777</v>
+      </c>
+      <c r="AU18" s="1" t="n">
+        <v>14075110863.4924</v>
+      </c>
+      <c r="AV18" s="1" t="n">
+        <v>5937071580.75196</v>
+      </c>
+      <c r="AW18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="M19" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1" t="n">
+        <v>12691072293.3044</v>
+      </c>
+      <c r="Z19" s="1" t="n">
+        <v>15022207352.4547</v>
+      </c>
+      <c r="AA19" s="1" t="n">
+        <v>16617986223.1623</v>
+      </c>
+      <c r="AB19" s="1" t="n">
+        <v>20821134455.0143</v>
+      </c>
+      <c r="AC19" s="1" t="n">
+        <v>21068557814.3519</v>
+      </c>
+      <c r="AD19" s="1" t="n">
+        <v>22956492567.2655</v>
+      </c>
+      <c r="AE19" s="1" t="n">
+        <v>25400822925.9006</v>
+      </c>
+      <c r="AF19" s="1" t="n">
+        <v>29499075103.2976</v>
+      </c>
+      <c r="AG19" s="1" t="n">
+        <v>29796228982.4389</v>
+      </c>
+      <c r="AH19" s="1" t="n">
+        <v>31831808039.0013</v>
+      </c>
+      <c r="AI19" s="1" t="n">
+        <v>31847844799.5056</v>
+      </c>
+      <c r="AJ19" s="1" t="n">
+        <v>28598299073.8855</v>
+      </c>
+      <c r="AK19" s="1" t="n">
+        <v>29698241444.6815</v>
+      </c>
+      <c r="AL19" s="1" t="n">
+        <v>20674966786.4464</v>
+      </c>
+      <c r="AM19" s="1" t="n">
+        <v>19896032822.361</v>
+      </c>
+      <c r="AN19" s="1" t="n">
+        <v>17738378432.7225</v>
+      </c>
+      <c r="AO19" s="1" t="n">
+        <v>20034518758.319</v>
+      </c>
+      <c r="AP19" s="1" t="n">
+        <v>20335264795.608</v>
+      </c>
+      <c r="AQ19" s="1" t="n">
+        <v>25954788224.6266</v>
+      </c>
+      <c r="AR19" s="1" t="n">
+        <v>28050576848.755</v>
+      </c>
+      <c r="AS19" s="1" t="n">
+        <v>34330459787.0265</v>
+      </c>
+      <c r="AT19" s="1" t="n">
+        <v>29374087100.7472</v>
+      </c>
+      <c r="AU19" s="1" t="n">
+        <v>27976052355.6285</v>
+      </c>
+      <c r="AV19" s="1" t="n">
+        <v>15180442495.459</v>
+      </c>
+      <c r="AW19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="M20" t="s">
+        <v>70</v>
+      </c>
+      <c r="N20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1" t="n">
+        <v>1855051009.96975</v>
+      </c>
+      <c r="Z20" s="1" t="n">
+        <v>390549561.296667</v>
+      </c>
+      <c r="AA20" s="1" t="n">
+        <v>265431127.071155</v>
+      </c>
+      <c r="AB20" s="1" t="n">
+        <v>270576760.86316</v>
+      </c>
+      <c r="AC20" s="1" t="n">
+        <v>144779797.65075</v>
+      </c>
+      <c r="AD20" s="1" t="n">
+        <v>181104602.230591</v>
+      </c>
+      <c r="AE20" s="1" t="n">
+        <v>47563684.0781634</v>
+      </c>
+      <c r="AF20" s="1" t="n">
+        <v>31446672.5264624</v>
+      </c>
+      <c r="AG20" s="1" t="n">
+        <v>10614134.3942582</v>
+      </c>
+      <c r="AH20" s="1" t="n">
+        <v>1153515.46896845</v>
+      </c>
+      <c r="AI20" s="1" t="n">
+        <v>318742516.203352</v>
+      </c>
+      <c r="AJ20" s="1" t="n">
+        <v>247359291.637774</v>
+      </c>
+      <c r="AK20" s="1" t="n">
+        <v>329466406.214043</v>
+      </c>
+      <c r="AL20" s="1" t="n">
+        <v>135987321.787702</v>
+      </c>
+      <c r="AM20" s="1" t="n">
+        <v>135489966.414784</v>
+      </c>
+      <c r="AN20" s="1" t="n">
+        <v>108986041.613053</v>
+      </c>
+      <c r="AO20" s="1" t="n">
+        <v>303855.428201114</v>
+      </c>
+      <c r="AP20" s="1" t="n">
+        <v>30511221.1232605</v>
+      </c>
+      <c r="AQ20" s="1" t="n">
+        <v>2204043.63422428</v>
+      </c>
+      <c r="AR20" s="1" t="n">
+        <v>32798.4707456821</v>
+      </c>
+      <c r="AS20" s="1" t="n">
+        <v>97772.0343696636</v>
+      </c>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21" s="1" t="n">
+        <v>81553023298.5625</v>
+      </c>
+      <c r="P21" s="1" t="n">
+        <v>83720006592.9594</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>72275362881.4491</v>
+      </c>
+      <c r="R21" s="1" t="n">
+        <v>72170931992.9669</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <v>77976219082.6946</v>
+      </c>
+      <c r="T21" s="1" t="n">
+        <v>65001740875.7447</v>
+      </c>
+      <c r="U21" s="1" t="n">
+        <v>67251730788.5116</v>
+      </c>
+      <c r="V21" s="1" t="n">
+        <v>59081351363.2833</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <v>56199563119.5895</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <v>58134071992.2562</v>
+      </c>
+      <c r="Y21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="2" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="N1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2" t="n">
+        <v>25037791820.28</v>
+      </c>
+      <c r="AA2" s="2" t="n">
+        <v>25987627628.125</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>30299261383.9775</v>
+      </c>
+      <c r="AC2" s="2" t="n">
+        <v>32207058151.3866</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>30328711951.8153</v>
+      </c>
+      <c r="AE2" s="2" t="n">
+        <v>27829791611.4059</v>
+      </c>
+      <c r="AF2" s="2" t="n">
+        <v>32177683976.4133</v>
+      </c>
+      <c r="AG2" s="2" t="n">
+        <v>34883515514.1267</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>31027929889.2513</v>
+      </c>
+      <c r="AI2" s="2" t="n">
+        <v>32875058064.4656</v>
+      </c>
+      <c r="AJ2" s="2" t="n">
+        <v>30416463887.6224</v>
+      </c>
+      <c r="AK2" s="2" t="n">
+        <v>32442032021.952</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>36243285201.6863</v>
+      </c>
+      <c r="AM2" s="2" t="n">
+        <v>28738866549.7774</v>
+      </c>
+      <c r="AN2" s="2" t="n">
+        <v>29224642112.3227</v>
+      </c>
+      <c r="AO2" s="2" t="n">
+        <v>26728714114.7883</v>
+      </c>
+      <c r="AP2" s="2" t="n">
+        <v>35382047605.571</v>
+      </c>
+      <c r="AQ2" s="2" t="n">
+        <v>28839227430.4421</v>
+      </c>
+      <c r="AR2" s="2" t="n">
+        <v>32185609526.1376</v>
+      </c>
+      <c r="AS2" s="2" t="n">
+        <v>32232730048.8324</v>
+      </c>
+      <c r="AT2" s="2" t="n">
+        <v>27888874191.2234</v>
+      </c>
+      <c r="AU2" s="2" t="n">
+        <v>32293940253.82</v>
+      </c>
+      <c r="AV2" s="2" t="n">
+        <v>29109738531.2029</v>
+      </c>
+      <c r="AW2" s="2" t="n">
+        <v>19266830668.5575</v>
+      </c>
+      <c r="AX2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="N3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="n">
+        <v>429991936</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>462457544</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>580716042.8604</v>
+      </c>
+      <c r="AC3" s="2" t="n">
+        <v>814693170.4201</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>699659535.1131</v>
+      </c>
+      <c r="AE3" s="2" t="n">
+        <v>905201048.2908</v>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>1009097304.2691</v>
+      </c>
+      <c r="AG3" s="2" t="n">
+        <v>1104709717.6857</v>
+      </c>
+      <c r="AH3" s="2" t="n">
+        <v>1031110140.2592</v>
+      </c>
+      <c r="AI3" s="2" t="n">
+        <v>1048622648.7144</v>
+      </c>
+      <c r="AJ3" s="2" t="n">
+        <v>993249631.0746</v>
+      </c>
+      <c r="AK3" s="2" t="n">
+        <v>974754574.7314</v>
+      </c>
+      <c r="AL3" s="2" t="n">
+        <v>754192638.8197</v>
+      </c>
+      <c r="AM3" s="2" t="n">
+        <v>585889371.8041</v>
+      </c>
+      <c r="AN3" s="2" t="n">
+        <v>708079176.1999</v>
+      </c>
+      <c r="AO3" s="2" t="n">
+        <v>654096032.3745</v>
+      </c>
+      <c r="AP3" s="2" t="n">
+        <v>718615400.6798</v>
+      </c>
+      <c r="AQ3" s="2" t="n">
+        <v>770474048.8266</v>
+      </c>
+      <c r="AR3" s="2" t="n">
+        <v>836529128.8416</v>
+      </c>
+      <c r="AS3" s="2" t="n">
+        <v>970251135.2166</v>
+      </c>
+      <c r="AT3" s="2" t="n">
+        <v>1059955437.244</v>
+      </c>
+      <c r="AU3" s="2" t="n">
+        <v>1378269878.9255</v>
+      </c>
+      <c r="AV3" s="2" t="n">
+        <v>1586761989.3851</v>
+      </c>
+      <c r="AW3" s="2" t="n">
+        <v>605325076.8962</v>
+      </c>
+      <c r="AX3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="N4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2" t="n">
+        <v>794993</v>
+      </c>
+      <c r="AA4" s="2" t="n">
+        <v>5766024</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>18457363</v>
+      </c>
+      <c r="AC4" s="2" t="n">
+        <v>21048810</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>8333396</v>
+      </c>
+      <c r="AE4" s="2" t="n">
+        <v>7380604</v>
+      </c>
+      <c r="AF4" s="2" t="n">
+        <v>8035145</v>
+      </c>
+      <c r="AG4" s="2" t="n">
+        <v>2593749.5782</v>
+      </c>
+      <c r="AH4" s="2" t="n">
+        <v>3037136.4004</v>
+      </c>
+      <c r="AI4" s="2" t="n">
+        <v>-191.57</v>
+      </c>
+      <c r="AJ4" s="2" t="n">
+        <v>80526041.4074</v>
+      </c>
+      <c r="AK4" s="2" t="n">
+        <v>1205687097.1125</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <v>3785228474.7754</v>
+      </c>
+      <c r="AM4" s="2" t="n">
+        <v>3588830488.7816</v>
+      </c>
+      <c r="AN4" s="2" t="n">
+        <v>3547464959.5712</v>
+      </c>
+      <c r="AO4" s="2" t="n">
+        <v>4158248013.9978</v>
+      </c>
+      <c r="AP4" s="2" t="n">
+        <v>4079140178.3866</v>
+      </c>
+      <c r="AQ4" s="2" t="n">
+        <v>4331574462.2964</v>
+      </c>
+      <c r="AR4" s="2" t="n">
+        <v>4814361963.939</v>
+      </c>
+      <c r="AS4" s="2" t="n">
+        <v>5165041167.6537</v>
+      </c>
+      <c r="AT4" s="2" t="n">
+        <v>4039210682.0812</v>
+      </c>
+      <c r="AU4" s="2" t="n">
+        <v>4181022951.238</v>
+      </c>
+      <c r="AV4" s="2" t="n">
+        <v>4135689645.2253</v>
+      </c>
+      <c r="AW4" s="2" t="n">
+        <v>2810193207.7628</v>
+      </c>
+      <c r="AX4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2" t="n">
+        <v>1167331912</v>
+      </c>
+      <c r="AA5" s="2" t="n">
+        <v>1676747428.4924</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>2117718162.5801</v>
+      </c>
+      <c r="AC5" s="2" t="n">
+        <v>2882510310.7922</v>
+      </c>
+      <c r="AD5" s="2" t="n">
+        <v>3000071367.2545</v>
+      </c>
+      <c r="AE5" s="2" t="n">
+        <v>3143873186.8138</v>
+      </c>
+      <c r="AF5" s="2" t="n">
+        <v>3315801109.2555</v>
+      </c>
+      <c r="AG5" s="2" t="n">
+        <v>2786606127.6962</v>
+      </c>
+      <c r="AH5" s="2" t="n">
+        <v>2397916048.7393</v>
+      </c>
+      <c r="AI5" s="2" t="n">
+        <v>2312431378.2869</v>
+      </c>
+      <c r="AJ5" s="2" t="n">
+        <v>1879357769.5313</v>
+      </c>
+      <c r="AK5" s="2" t="n">
+        <v>1578069327.0811</v>
+      </c>
+      <c r="AL5" s="2" t="n">
+        <v>1462436345.3911</v>
+      </c>
+      <c r="AM5" s="2" t="n">
+        <v>964787397.5667</v>
+      </c>
+      <c r="AN5" s="2" t="n">
+        <v>1259044409.1743</v>
+      </c>
+      <c r="AO5" s="2" t="n">
+        <v>993691370.6567</v>
+      </c>
+      <c r="AP5" s="2" t="n">
+        <v>1221989460.6681</v>
+      </c>
+      <c r="AQ5" s="2" t="n">
+        <v>1064078503.0135</v>
+      </c>
+      <c r="AR5" s="2" t="n">
+        <v>1342936841.4755</v>
+      </c>
+      <c r="AS5" s="2" t="n">
+        <v>1389286463.4796</v>
+      </c>
+      <c r="AT5" s="2" t="n">
+        <v>2176356701.8175</v>
+      </c>
+      <c r="AU5" s="2" t="n">
+        <v>1985876952.3088</v>
+      </c>
+      <c r="AV5" s="2" t="n">
+        <v>2086575759.0228</v>
+      </c>
+      <c r="AW5" s="2" t="n">
+        <v>881360650.0195</v>
+      </c>
+      <c r="AX5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2" t="n">
+        <v>2320173951</v>
+      </c>
+      <c r="AA6" s="2" t="n">
+        <v>2729937455</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>3526006911.2676</v>
+      </c>
+      <c r="AC6" s="2" t="n">
+        <v>5790650834.9219</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>6758654015.125</v>
+      </c>
+      <c r="AE6" s="2" t="n">
+        <v>7666611064.2898</v>
+      </c>
+      <c r="AF6" s="2" t="n">
+        <v>8427156969.5412</v>
+      </c>
+      <c r="AG6" s="2" t="n">
+        <v>9399128455.1433</v>
+      </c>
+      <c r="AH6" s="2" t="n">
+        <v>6830206594.959</v>
+      </c>
+      <c r="AI6" s="2" t="n">
+        <v>7451026417.8535</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>6948176906.6676</v>
+      </c>
+      <c r="AK6" s="2" t="n">
+        <v>6777124492.4024</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>5403440476.1178</v>
+      </c>
+      <c r="AM6" s="2" t="n">
+        <v>4355883264.0082</v>
+      </c>
+      <c r="AN6" s="2" t="n">
+        <v>4557892835.049</v>
+      </c>
+      <c r="AO6" s="2" t="n">
+        <v>5546452743.2363</v>
+      </c>
+      <c r="AP6" s="2" t="n">
+        <v>6844533124.3459</v>
+      </c>
+      <c r="AQ6" s="2" t="n">
+        <v>8572838086.3563</v>
+      </c>
+      <c r="AR6" s="2" t="n">
+        <v>9431813502.821</v>
+      </c>
+      <c r="AS6" s="2" t="n">
+        <v>11043379299.655</v>
+      </c>
+      <c r="AT6" s="2" t="n">
+        <v>11792177479.1521</v>
+      </c>
+      <c r="AU6" s="2" t="n">
+        <v>11743892048.6738</v>
+      </c>
+      <c r="AV6" s="2" t="n">
+        <v>14075110863.4924</v>
+      </c>
+      <c r="AW6" s="2" t="n">
+        <v>6224661006.7286</v>
+      </c>
+      <c r="AX6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="N7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2" t="n">
+        <v>7854698435</v>
+      </c>
+      <c r="AA7" s="2" t="n">
+        <v>9522931884.9922</v>
+      </c>
+      <c r="AB7" s="2" t="n">
+        <v>10700806025.8984</v>
+      </c>
+      <c r="AC7" s="2" t="n">
+        <v>13663611137.4668</v>
+      </c>
+      <c r="AD7" s="2" t="n">
+        <v>14163933177.4563</v>
+      </c>
+      <c r="AE7" s="2" t="n">
+        <v>15901650491.4803</v>
+      </c>
+      <c r="AF7" s="2" t="n">
+        <v>18167649663.3896</v>
+      </c>
+      <c r="AG7" s="2" t="n">
+        <v>21677474869.1647</v>
+      </c>
+      <c r="AH7" s="2" t="n">
+        <v>22352495458.8577</v>
+      </c>
+      <c r="AI7" s="2" t="n">
+        <v>24122206299.4763</v>
+      </c>
+      <c r="AJ7" s="2" t="n">
+        <v>24344266986.4574</v>
+      </c>
+      <c r="AK7" s="2" t="n">
+        <v>22300905029.3058</v>
+      </c>
+      <c r="AL7" s="2" t="n">
+        <v>23583134638.5674</v>
+      </c>
+      <c r="AM7" s="2" t="n">
+        <v>16718271014.0538</v>
+      </c>
+      <c r="AN7" s="2" t="n">
+        <v>16399652239.6038</v>
+      </c>
+      <c r="AO7" s="2" t="n">
+        <v>14788790206.1206</v>
+      </c>
+      <c r="AP7" s="2" t="n">
+        <v>16841532236.8939</v>
+      </c>
+      <c r="AQ7" s="2" t="n">
+        <v>17399545625.617</v>
+      </c>
+      <c r="AR7" s="2" t="n">
+        <v>22729246769.6889</v>
+      </c>
+      <c r="AS7" s="2" t="n">
+        <v>25045714764.7329</v>
+      </c>
+      <c r="AT7" s="2" t="n">
+        <v>31061800889.3761</v>
+      </c>
+      <c r="AU7" s="2" t="n">
+        <v>27470707824.7053</v>
+      </c>
+      <c r="AV7" s="2" t="n">
+        <v>27976052355.6285</v>
+      </c>
+      <c r="AW7" s="2" t="n">
+        <v>15915777194.386</v>
+      </c>
+      <c r="AX7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="N8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2" t="n">
+        <v>1148119396.6992</v>
+      </c>
+      <c r="AA8" s="2" t="n">
+        <v>247578587</v>
+      </c>
+      <c r="AB8" s="2" t="n">
+        <v>170918844.5508</v>
+      </c>
+      <c r="AC8" s="2" t="n">
+        <v>177562642</v>
+      </c>
+      <c r="AD8" s="2" t="n">
+        <v>97332309</v>
+      </c>
+      <c r="AE8" s="2" t="n">
+        <v>125448697.2969</v>
+      </c>
+      <c r="AF8" s="2" t="n">
+        <v>34019384</v>
+      </c>
+      <c r="AG8" s="2" t="n">
+        <v>23108672.0863</v>
+      </c>
+      <c r="AH8" s="2" t="n">
+        <v>7962497.2337</v>
+      </c>
+      <c r="AI8" s="2" t="n">
+        <v>874136.2752</v>
+      </c>
+      <c r="AJ8" s="2" t="n">
+        <v>243644521.7326</v>
+      </c>
+      <c r="AK8" s="2" t="n">
+        <v>192890355.3557</v>
+      </c>
+      <c r="AL8" s="2" t="n">
+        <v>261626622.9468</v>
+      </c>
+      <c r="AM8" s="2" t="n">
+        <v>109962590.1993</v>
+      </c>
+      <c r="AN8" s="2" t="n">
+        <v>111679969.1173</v>
+      </c>
+      <c r="AO8" s="2" t="n">
+        <v>90863531.3495</v>
+      </c>
+      <c r="AP8" s="2" t="n">
+        <v>255428.6954</v>
+      </c>
+      <c r="AQ8" s="2" t="n">
+        <v>26106440.6765</v>
+      </c>
+      <c r="AR8" s="2" t="n">
+        <v>1930135.2498</v>
+      </c>
+      <c r="AS8" s="2" t="n">
+        <v>29285</v>
+      </c>
+      <c r="AT8" s="2" t="n">
+        <v>88463</v>
+      </c>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9" s="2" t="n">
+        <v>41032316000</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>43625084000</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>38602723036</v>
+      </c>
+      <c r="S9" s="2" t="n">
+        <v>39452449414</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>43554730825</v>
+      </c>
+      <c r="U9" s="2" t="n">
+        <v>37076749369</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>39081089944</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>34943056076</v>
+      </c>
+      <c r="X9" s="2" t="n">
+        <v>33653688998</v>
+      </c>
+      <c r="Y9" s="2" t="n">
+        <v>35246060466</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="2"/>
+    </row>
+    <row r="13">
+      <c r="N13" t="s">
+        <v>65</v>
+      </c>
+      <c r="O13" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" t="s">
+        <v>5</v>
+      </c>
+      <c r="U13" t="s">
+        <v>6</v>
+      </c>
+      <c r="V13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="N14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2" t="n">
+        <v>40454312623.8912</v>
+      </c>
+      <c r="AA14" s="2" t="n">
+        <v>40994888501.0211</v>
+      </c>
+      <c r="AB14" s="2" t="n">
+        <v>47053717919.2218</v>
+      </c>
+      <c r="AC14" s="2" t="n">
+        <v>49078349890.365</v>
+      </c>
+      <c r="AD14" s="2" t="n">
+        <v>45113332093.9883</v>
+      </c>
+      <c r="AE14" s="2" t="n">
+        <v>40176609630.433</v>
+      </c>
+      <c r="AF14" s="2" t="n">
+        <v>44988739214.7108</v>
+      </c>
+      <c r="AG14" s="2" t="n">
+        <v>47470078975.0205</v>
+      </c>
+      <c r="AH14" s="2" t="n">
+        <v>41360719904.0871</v>
+      </c>
+      <c r="AI14" s="2" t="n">
+        <v>43382123699.1001</v>
+      </c>
+      <c r="AJ14" s="2" t="n">
+        <v>39791661083.1474</v>
+      </c>
+      <c r="AK14" s="2" t="n">
+        <v>41603106829.4826</v>
+      </c>
+      <c r="AL14" s="2" t="n">
+        <v>45641169045.7752</v>
+      </c>
+      <c r="AM14" s="2" t="n">
+        <v>35540464136.3503</v>
+      </c>
+      <c r="AN14" s="2" t="n">
+        <v>35455290770.3958</v>
+      </c>
+      <c r="AO14" s="2" t="n">
+        <v>32059691116.0415</v>
+      </c>
+      <c r="AP14" s="2" t="n">
+        <v>42090130903.2132</v>
+      </c>
+      <c r="AQ14" s="2" t="n">
+        <v>33705094312.0825</v>
+      </c>
+      <c r="AR14" s="2" t="n">
+        <v>36753117584.409</v>
+      </c>
+      <c r="AS14" s="2" t="n">
+        <v>36099854996.0764</v>
+      </c>
+      <c r="AT14" s="2" t="n">
+        <v>30823643398.4323</v>
+      </c>
+      <c r="AU14" s="2" t="n">
+        <v>34531509704.6361</v>
+      </c>
+      <c r="AV14" s="2" t="n">
+        <v>29109738531.2029</v>
+      </c>
+      <c r="AW14" s="2" t="n">
+        <v>18376671868.5249</v>
+      </c>
+      <c r="AX14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="N15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2" t="n">
+        <v>694750892.153622</v>
+      </c>
+      <c r="AA15" s="2" t="n">
+        <v>729516203.788391</v>
+      </c>
+      <c r="AB15" s="2" t="n">
+        <v>901832177.545081</v>
+      </c>
+      <c r="AC15" s="2" t="n">
+        <v>1241460684.89795</v>
+      </c>
+      <c r="AD15" s="2" t="n">
+        <v>1040729095.59859</v>
+      </c>
+      <c r="AE15" s="2" t="n">
+        <v>1306797753.35914</v>
+      </c>
+      <c r="AF15" s="2" t="n">
+        <v>1410854040.87216</v>
+      </c>
+      <c r="AG15" s="2" t="n">
+        <v>1503307701.93663</v>
+      </c>
+      <c r="AH15" s="2" t="n">
+        <v>1374486079.27591</v>
+      </c>
+      <c r="AI15" s="2" t="n">
+        <v>1383768733.45746</v>
+      </c>
+      <c r="AJ15" s="2" t="n">
+        <v>1299396696.36499</v>
+      </c>
+      <c r="AK15" s="2" t="n">
+        <v>1250008590.01795</v>
+      </c>
+      <c r="AL15" s="2" t="n">
+        <v>949754789.884435</v>
+      </c>
+      <c r="AM15" s="2" t="n">
+        <v>724551198.649611</v>
+      </c>
+      <c r="AN15" s="2" t="n">
+        <v>859040565.292127</v>
+      </c>
+      <c r="AO15" s="2" t="n">
+        <v>784553894.665383</v>
+      </c>
+      <c r="AP15" s="2" t="n">
+        <v>854857712.613427</v>
+      </c>
+      <c r="AQ15" s="2" t="n">
+        <v>900471434.033643</v>
+      </c>
+      <c r="AR15" s="2" t="n">
+        <v>955242230.541908</v>
+      </c>
+      <c r="AS15" s="2" t="n">
+        <v>1086657110.27374</v>
+      </c>
+      <c r="AT15" s="2" t="n">
+        <v>1171495421.14254</v>
+      </c>
+      <c r="AU15" s="2" t="n">
+        <v>1473766883.99285</v>
+      </c>
+      <c r="AV15" s="2" t="n">
+        <v>1586761989.3851</v>
+      </c>
+      <c r="AW15" s="2" t="n">
+        <v>577358077.375156</v>
+      </c>
+      <c r="AX15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="N16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2" t="n">
+        <v>1284494.07945614</v>
+      </c>
+      <c r="AA16" s="2" t="n">
+        <v>9095771.04754237</v>
+      </c>
+      <c r="AB16" s="2" t="n">
+        <v>28663654.2432003</v>
+      </c>
+      <c r="AC16" s="2" t="n">
+        <v>32074983.5983185</v>
+      </c>
+      <c r="AD16" s="2" t="n">
+        <v>12395754.2877521</v>
+      </c>
+      <c r="AE16" s="2" t="n">
+        <v>10655043.6986845</v>
+      </c>
+      <c r="AF16" s="2" t="n">
+        <v>11234215.7136718</v>
+      </c>
+      <c r="AG16" s="2" t="n">
+        <v>3529618.37429253</v>
+      </c>
+      <c r="AH16" s="2" t="n">
+        <v>4048550.72239184</v>
+      </c>
+      <c r="AI16" s="2" t="n">
+        <v>-252.796920411209</v>
+      </c>
+      <c r="AJ16" s="2" t="n">
+        <v>105346399.235931</v>
+      </c>
+      <c r="AK16" s="2" t="n">
+        <v>1546152505.80355</v>
+      </c>
+      <c r="AL16" s="2" t="n">
+        <v>4766738217.37517</v>
+      </c>
+      <c r="AM16" s="2" t="n">
+        <v>4438195259.26888</v>
+      </c>
+      <c r="AN16" s="2" t="n">
+        <v>4303779021.68914</v>
+      </c>
+      <c r="AO16" s="2" t="n">
+        <v>4987600463.68652</v>
+      </c>
+      <c r="AP16" s="2" t="n">
+        <v>4852504467.65594</v>
+      </c>
+      <c r="AQ16" s="2" t="n">
+        <v>5062414592.19526</v>
+      </c>
+      <c r="AR16" s="2" t="n">
+        <v>5497575281.61345</v>
+      </c>
+      <c r="AS16" s="2" t="n">
+        <v>5784717488.04963</v>
+      </c>
+      <c r="AT16" s="2" t="n">
+        <v>4464260149.83389</v>
+      </c>
+      <c r="AU16" s="2" t="n">
+        <v>4470715975.85256</v>
+      </c>
+      <c r="AV16" s="2" t="n">
+        <v>4135689645.2253</v>
+      </c>
+      <c r="AW16" s="2" t="n">
+        <v>2680357727.4643</v>
+      </c>
+      <c r="AX16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="N17" t="s">
+        <v>70</v>
+      </c>
+      <c r="O17" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2" t="n">
+        <v>1886093248.2729</v>
+      </c>
+      <c r="AA17" s="2" t="n">
+        <v>2645030737.66642</v>
+      </c>
+      <c r="AB17" s="2" t="n">
+        <v>3288743966.12027</v>
+      </c>
+      <c r="AC17" s="2" t="n">
+        <v>4392479714.56076</v>
+      </c>
+      <c r="AD17" s="2" t="n">
+        <v>4462544143.37293</v>
+      </c>
+      <c r="AE17" s="2" t="n">
+        <v>4538667321.62076</v>
+      </c>
+      <c r="AF17" s="2" t="n">
+        <v>4635936865.48388</v>
+      </c>
+      <c r="AG17" s="2" t="n">
+        <v>3792060834.59235</v>
+      </c>
+      <c r="AH17" s="2" t="n">
+        <v>3196459912.06713</v>
+      </c>
+      <c r="AI17" s="2" t="n">
+        <v>3051498309.1986</v>
+      </c>
+      <c r="AJ17" s="2" t="n">
+        <v>2458627922.54432</v>
+      </c>
+      <c r="AK17" s="2" t="n">
+        <v>2023689106.60284</v>
+      </c>
+      <c r="AL17" s="2" t="n">
+        <v>1841646089.39963</v>
+      </c>
+      <c r="AM17" s="2" t="n">
+        <v>1193122625.17492</v>
+      </c>
+      <c r="AN17" s="2" t="n">
+        <v>1527470736.80308</v>
+      </c>
+      <c r="AO17" s="2" t="n">
+        <v>1191880696.95818</v>
+      </c>
+      <c r="AP17" s="2" t="n">
+        <v>1453666473.32668</v>
+      </c>
+      <c r="AQ17" s="2" t="n">
+        <v>1243613976.34637</v>
+      </c>
+      <c r="AR17" s="2" t="n">
+        <v>1533515020.21739</v>
+      </c>
+      <c r="AS17" s="2" t="n">
+        <v>1555966243.12132</v>
+      </c>
+      <c r="AT17" s="2" t="n">
+        <v>2405376510.52698</v>
+      </c>
+      <c r="AU17" s="2" t="n">
+        <v>2123473590.14987</v>
+      </c>
+      <c r="AV17" s="2" t="n">
+        <v>2086575759.0228</v>
+      </c>
+      <c r="AW17" s="2" t="n">
+        <v>840640359.686659</v>
+      </c>
+      <c r="AX17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="N18" t="s">
+        <v>70</v>
+      </c>
+      <c r="O18" t="s">
+        <v>73</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2" t="n">
+        <v>3748774773.32236</v>
+      </c>
+      <c r="AA18" s="2" t="n">
+        <v>4306413928.34829</v>
+      </c>
+      <c r="AB18" s="2" t="n">
+        <v>5475768286.27736</v>
+      </c>
+      <c r="AC18" s="2" t="n">
+        <v>8824015730.7567</v>
+      </c>
+      <c r="AD18" s="2" t="n">
+        <v>10053358137.2371</v>
+      </c>
+      <c r="AE18" s="2" t="n">
+        <v>11067939143.033</v>
+      </c>
+      <c r="AF18" s="2" t="n">
+        <v>11782301283.7725</v>
+      </c>
+      <c r="AG18" s="2" t="n">
+        <v>12790493259.8128</v>
+      </c>
+      <c r="AH18" s="2" t="n">
+        <v>9104773114.72243</v>
+      </c>
+      <c r="AI18" s="2" t="n">
+        <v>9832419127.92154</v>
+      </c>
+      <c r="AJ18" s="2" t="n">
+        <v>9089797605.57828</v>
+      </c>
+      <c r="AK18" s="2" t="n">
+        <v>8690868502.42111</v>
+      </c>
+      <c r="AL18" s="2" t="n">
+        <v>6804552590.27684</v>
+      </c>
+      <c r="AM18" s="2" t="n">
+        <v>5386785615.16933</v>
+      </c>
+      <c r="AN18" s="2" t="n">
+        <v>5529628562.9731</v>
+      </c>
+      <c r="AO18" s="2" t="n">
+        <v>6652679248.77445</v>
+      </c>
+      <c r="AP18" s="2" t="n">
+        <v>8142188331.96465</v>
+      </c>
+      <c r="AQ18" s="2" t="n">
+        <v>10019280749.4504</v>
+      </c>
+      <c r="AR18" s="2" t="n">
+        <v>10770296284.8004</v>
+      </c>
+      <c r="AS18" s="2" t="n">
+        <v>12368309813.6659</v>
+      </c>
+      <c r="AT18" s="2" t="n">
+        <v>13033078030.1915</v>
+      </c>
+      <c r="AU18" s="2" t="n">
+        <v>12557598083.777</v>
+      </c>
+      <c r="AV18" s="2" t="n">
+        <v>14075110863.4924</v>
+      </c>
+      <c r="AW18" s="2" t="n">
+        <v>5937071580.75196</v>
+      </c>
+      <c r="AX18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="N19" t="s">
+        <v>70</v>
+      </c>
+      <c r="O19" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2" t="n">
+        <v>12691072293.3044</v>
+      </c>
+      <c r="AA19" s="2" t="n">
+        <v>15022207352.4547</v>
+      </c>
+      <c r="AB19" s="2" t="n">
+        <v>16617986223.1623</v>
+      </c>
+      <c r="AC19" s="2" t="n">
+        <v>20821134455.0143</v>
+      </c>
+      <c r="AD19" s="2" t="n">
+        <v>21068557814.3519</v>
+      </c>
+      <c r="AE19" s="2" t="n">
+        <v>22956492567.2655</v>
+      </c>
+      <c r="AF19" s="2" t="n">
+        <v>25400822925.9006</v>
+      </c>
+      <c r="AG19" s="2" t="n">
+        <v>29499075103.2976</v>
+      </c>
+      <c r="AH19" s="2" t="n">
+        <v>29796228982.4389</v>
+      </c>
+      <c r="AI19" s="2" t="n">
+        <v>31831808039.0013</v>
+      </c>
+      <c r="AJ19" s="2" t="n">
+        <v>31847844799.5056</v>
+      </c>
+      <c r="AK19" s="2" t="n">
+        <v>28598299073.8855</v>
+      </c>
+      <c r="AL19" s="2" t="n">
+        <v>29698241444.6815</v>
+      </c>
+      <c r="AM19" s="2" t="n">
+        <v>20674966786.4464</v>
+      </c>
+      <c r="AN19" s="2" t="n">
+        <v>19896032822.361</v>
+      </c>
+      <c r="AO19" s="2" t="n">
+        <v>17738378432.7225</v>
+      </c>
+      <c r="AP19" s="2" t="n">
+        <v>20034518758.319</v>
+      </c>
+      <c r="AQ19" s="2" t="n">
+        <v>20335264795.608</v>
+      </c>
+      <c r="AR19" s="2" t="n">
+        <v>25954788224.6266</v>
+      </c>
+      <c r="AS19" s="2" t="n">
+        <v>28050576848.755</v>
+      </c>
+      <c r="AT19" s="2" t="n">
+        <v>34330459787.0265</v>
+      </c>
+      <c r="AU19" s="2" t="n">
+        <v>29374087100.7472</v>
+      </c>
+      <c r="AV19" s="2" t="n">
+        <v>27976052355.6285</v>
+      </c>
+      <c r="AW19" s="2" t="n">
+        <v>15180442495.459</v>
+      </c>
+      <c r="AX19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="N20" t="s">
+        <v>70</v>
+      </c>
+      <c r="O20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2" t="n">
+        <v>1855051009.96975</v>
+      </c>
+      <c r="AA20" s="2" t="n">
+        <v>390549561.296667</v>
+      </c>
+      <c r="AB20" s="2" t="n">
+        <v>265431127.071155</v>
+      </c>
+      <c r="AC20" s="2" t="n">
+        <v>270576760.86316</v>
+      </c>
+      <c r="AD20" s="2" t="n">
+        <v>144779797.65075</v>
+      </c>
+      <c r="AE20" s="2" t="n">
+        <v>181104602.230591</v>
+      </c>
+      <c r="AF20" s="2" t="n">
+        <v>47563684.0781634</v>
+      </c>
+      <c r="AG20" s="2" t="n">
+        <v>31446672.5264624</v>
+      </c>
+      <c r="AH20" s="2" t="n">
+        <v>10614134.3942582</v>
+      </c>
+      <c r="AI20" s="2" t="n">
+        <v>1153515.46896845</v>
+      </c>
+      <c r="AJ20" s="2" t="n">
+        <v>318742516.203352</v>
+      </c>
+      <c r="AK20" s="2" t="n">
+        <v>247359291.637774</v>
+      </c>
+      <c r="AL20" s="2" t="n">
+        <v>329466406.214043</v>
+      </c>
+      <c r="AM20" s="2" t="n">
+        <v>135987321.787702</v>
+      </c>
+      <c r="AN20" s="2" t="n">
+        <v>135489966.414784</v>
+      </c>
+      <c r="AO20" s="2" t="n">
+        <v>108986041.613053</v>
+      </c>
+      <c r="AP20" s="2" t="n">
+        <v>303855.428201114</v>
+      </c>
+      <c r="AQ20" s="2" t="n">
+        <v>30511221.1232605</v>
+      </c>
+      <c r="AR20" s="2" t="n">
+        <v>2204043.63422428</v>
+      </c>
+      <c r="AS20" s="2" t="n">
+        <v>32798.4707456821</v>
+      </c>
+      <c r="AT20" s="2" t="n">
+        <v>97772.0343696636</v>
+      </c>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21" s="2" t="n">
+        <v>81553023298.5625</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>83720006592.9594</v>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>72275362881.4491</v>
+      </c>
+      <c r="S21" s="2" t="n">
+        <v>72170931992.9669</v>
+      </c>
+      <c r="T21" s="2" t="n">
+        <v>77976219082.6946</v>
+      </c>
+      <c r="U21" s="2" t="n">
+        <v>65001740875.7447</v>
+      </c>
+      <c r="V21" s="2" t="n">
+        <v>67251730788.5116</v>
+      </c>
+      <c r="W21" s="2" t="n">
+        <v>59081351363.2833</v>
+      </c>
+      <c r="X21" s="2" t="n">
+        <v>56199563119.5895</v>
+      </c>
+      <c r="Y21" s="2" t="n">
+        <v>58134071992.2562</v>
+      </c>
+      <c r="Z21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>